<commit_message>
Nuevo release de operaciones adecuado a reunión del martes 15 de junio con Mtra Gianni.
</commit_message>
<xml_diff>
--- a/database/datafiles/plantilla_reporte_operativo.xlsx
+++ b/database/datafiles/plantilla_reporte_operativo.xlsx
@@ -196,7 +196,7 @@
     <t xml:space="preserve">Número de pagos/Convenios totales</t>
   </si>
   <si>
-    <t xml:space="preserve">Del total de Convenios Diferidos y Parciales</t>
+    <t xml:space="preserve">Del total de Convenios Diferidos</t>
   </si>
   <si>
     <t xml:space="preserve">Constancias de no conciliación</t>
@@ -818,8 +818,8 @@
   </sheetPr>
   <dimension ref="A1:V93"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O2" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U10" activeCellId="0" sqref="U10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P3" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S11" activeCellId="0" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1000,7 +1000,6 @@
         <v>22</v>
       </c>
       <c r="B4" s="4" t="n">
-        <f aca="false">B5-B2-B3</f>
         <v>0</v>
       </c>
       <c r="C4" s="4"/>
@@ -1277,15 +1276,12 @@
         <v>57</v>
       </c>
       <c r="T9" s="27" t="n">
-        <f aca="false">SUM(T7:T8)</f>
         <v>0</v>
       </c>
       <c r="U9" s="27" t="n">
-        <f aca="false">SUM(U7:U8)</f>
         <v>0</v>
       </c>
       <c r="V9" s="40" t="n">
-        <f aca="false">SUM(V7:V8)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se agregan indicadores por centro y por conciliador
</commit_message>
<xml_diff>
--- a/database/datafiles/plantilla_reporte_operativo.xlsx
+++ b/database/datafiles/plantilla_reporte_operativo.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Indicadores por centro" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="101">
   <si>
     <t xml:space="preserve">1. Solicitudes </t>
   </si>
@@ -145,99 +146,102 @@
     <t xml:space="preserve">Solicitudes por concepto (total, confirmadas, no confirmadas y por confirmar)</t>
   </si>
   <si>
+    <t xml:space="preserve">PRESENTADAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONFIRMADAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARCHIVADAS POR NO CONFIRMACIÓN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POR CONFIRMAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Número de Ratificaciones </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Número de citatorios notificados por el solicitante</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Otras Audiencias </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Número de Pagos/Convenios Diferidos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presentadas por el trabajador</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monto de Ratificaciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Número de citatorios notificados por personal del CFCRL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Número de pagos/Convenios a la firma del convenio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presentadas por el patrón</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beneficios o prestaciones no económicas derivadas de ratificaciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Número de citatorios notificados por personal del CFCRL en compañía del solicitante</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ratificaciones de Convenio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Número de pagos/Convenios totales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Del total de Convenios Diferidos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Constancias de no conciliación</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Número de cumplimientos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Con asistencia del personal del CFCRL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Archivos por falta de Interés</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Número de incumplimientos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presentadas por los usuarios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Audiencias Diferidas </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pagos vencidos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cumplimientos de Convenio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pagos vigentes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incumplimientos de Convenio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hombre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mujer</t>
+  </si>
+  <si>
     <t xml:space="preserve">TOTAL</t>
   </si>
   <si>
-    <t xml:space="preserve">CONFIRMADAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARCHIVADAS POR NO CONFIRMACIÓN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">POR CONFIRMAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Número de Ratificaciones </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Número de citatorios notificados por el solicitante</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Otras Audiencias </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Número de Pagos/Convenios Diferidos </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Presentadas por el trabajador</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monto de Ratificaciones</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Número de citatorios notificados por personal del CFCRL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Número de pagos/Convenios a la firma del convenio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Presentadas por el patrón</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beneficios o prestaciones no económicas derivadas de ratificaciones</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Número de citatorios notificados por personal del CFCRL en compañía del solicitante</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ratificaciones de Convenio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Número de pagos/Convenios totales</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Del total de Convenios Diferidos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Constancias de no conciliación</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Número de cumplimientos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Con asistencia del personal del CFCRL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Archivos por falta de Interés</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Número de incumplimientos </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Presentadas por los usuarios</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Audiencias Diferidas </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pagos vencidos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cumplimientos de Convenio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pagos vigentes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Incumplimientos de Convenio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hombre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mujer</t>
-  </si>
-  <si>
     <t xml:space="preserve">De 18 a 19 años</t>
   </si>
   <si>
@@ -281,6 +285,45 @@
   </si>
   <si>
     <t xml:space="preserve">De 85 años a 89 años</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Centro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Convenio conciliación normal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Constancia no conciliación normal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAMOAE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SLP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZAC</t>
   </si>
 </sst>
 </file>
@@ -289,15 +332,14 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="_-\$* #,##0.00_-;&quot;-$&quot;* #,##0.00_-;_-\$* \-??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="&quot; $&quot;* #,##0.00\ ;&quot;-$&quot;* #,##0.00\ ;&quot; $&quot;* \-#\ ;\ @\ "/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -316,11 +358,87 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF0000EE"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="14"/>
       <color rgb="FFFFFFFF"/>
       <name val="Montserrat"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -328,7 +446,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -336,14 +453,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -351,7 +466,6 @@
       <color rgb="FFFFFFFF"/>
       <name val="Montserrat"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -359,7 +473,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -367,7 +480,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -375,22 +487,62 @@
       <color rgb="FFFFFFFF"/>
       <name val="Montserrat"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFE2EFD9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFFADEDE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF666699"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFD8D8D8"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -401,13 +553,13 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFADEDE"/>
-        <bgColor rgb="FFE2EFD9"/>
+        <bgColor rgb="FFFFCCCC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD9E2F3"/>
-        <bgColor rgb="FFD8D8D8"/>
+        <bgColor rgb="FFDDDDDD"/>
       </patternFill>
     </fill>
     <fill>
@@ -419,7 +571,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD8D8D8"/>
-        <bgColor rgb="FFD9E2F3"/>
+        <bgColor rgb="FFDDDDDD"/>
       </patternFill>
     </fill>
     <fill>
@@ -467,16 +619,31 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF3B7B7"/>
-        <bgColor rgb="FFFF99CC"/>
+        <bgColor rgb="FFFFCCCC"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -515,7 +682,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -541,109 +708,160 @@
     </xf>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="11" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="12" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="13" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="13" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="16" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="16" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="17" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="17" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="18" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="18" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="18" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="19" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="19" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="6" borderId="1" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="17" fillId="13" borderId="2" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -651,7 +869,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="13" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -667,55 +885,55 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="13" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="20" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="12" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="12" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="11" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="18" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="17" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="14" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="21" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="13" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="6" borderId="1" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="17" fillId="13" borderId="2" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="10" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="4" borderId="1" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="17" fillId="11" borderId="2" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -723,53 +941,78 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="21" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="13" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="23">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Heading" xfId="20"/>
+    <cellStyle name="Heading 1" xfId="21"/>
+    <cellStyle name="Heading 2" xfId="22"/>
+    <cellStyle name="Text" xfId="23"/>
+    <cellStyle name="Note" xfId="24"/>
+    <cellStyle name="Footnote" xfId="25"/>
+    <cellStyle name="Hyperlink" xfId="26"/>
+    <cellStyle name="Status" xfId="27"/>
+    <cellStyle name="Good" xfId="28"/>
+    <cellStyle name="Neutral" xfId="29"/>
+    <cellStyle name="Bad" xfId="30"/>
+    <cellStyle name="Warning" xfId="31"/>
+    <cellStyle name="Error" xfId="32"/>
+    <cellStyle name="Accent" xfId="33"/>
+    <cellStyle name="Accent 1" xfId="34"/>
+    <cellStyle name="Accent 2" xfId="35"/>
+    <cellStyle name="Accent 3" xfId="36"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFCC0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF0000EE"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF006600"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF996600"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFBFBFBF"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF8EAADB"/>
       <rgbColor rgb="FF9D2449"/>
-      <rgbColor rgb="FFFADEDE"/>
-      <rgbColor rgb="FFD9E2F3"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFE2EFD9"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
@@ -783,16 +1026,16 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFD9E2F3"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFADEDE"/>
       <rgbColor rgb="FFD8D8D8"/>
-      <rgbColor rgb="FFE2EFD9"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FFA8D08D"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFF3B7B7"/>
+      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FFFFCCCC"/>
       <rgbColor rgb="FF4472C4"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFA8D08D"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
@@ -818,8 +1061,8 @@
   </sheetPr>
   <dimension ref="A1:V93"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P3" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S11" activeCellId="0" sqref="S11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1564,7 +1807,7 @@
     </row>
     <row r="18" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="48" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="B18" s="4" t="n">
         <f aca="false">SUM(B16:B17)</f>
@@ -1621,7 +1864,7 @@
       <c r="T19" s="28"/>
       <c r="U19" s="28"/>
     </row>
-    <row r="20" customFormat="false" ht="34.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="33.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="36" t="s">
         <v>40</v>
       </c>
@@ -1656,7 +1899,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="48" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B21" s="4" t="n">
         <v>0</v>
@@ -1689,7 +1932,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="48" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B22" s="4" t="n">
         <v>0</v>
@@ -1722,7 +1965,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="48" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B23" s="4" t="n">
         <v>0</v>
@@ -1755,7 +1998,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="48" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B24" s="4" t="n">
         <v>0</v>
@@ -1788,7 +2031,7 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="48" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B25" s="4" t="n">
         <v>0</v>
@@ -1821,7 +2064,7 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="48" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B26" s="4" t="n">
         <v>0</v>
@@ -1854,7 +2097,7 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="48" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B27" s="4" t="n">
         <v>0</v>
@@ -1887,7 +2130,7 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="48" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B28" s="4" t="n">
         <v>0</v>
@@ -1920,7 +2163,7 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="48" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B29" s="4" t="n">
         <v>0</v>
@@ -1953,7 +2196,7 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="48" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B30" s="4" t="n">
         <v>0</v>
@@ -1986,7 +2229,7 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="48" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B31" s="4" t="n">
         <v>0</v>
@@ -2019,7 +2262,7 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="48" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B32" s="4" t="n">
         <v>0</v>
@@ -2052,7 +2295,7 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="48" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B33" s="4" t="n">
         <v>0</v>
@@ -2085,7 +2328,7 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="48" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B34" s="4" t="n">
         <v>0</v>
@@ -2118,7 +2361,7 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="48" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B35" s="4" t="n">
         <v>0</v>
@@ -3261,4 +3504,253 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F15"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="49"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+    </row>
+    <row r="2" customFormat="false" ht="46.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="49"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="B9" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="B11" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="49"/>
+      <c r="B14" s="49"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="49"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Arial,Regular"&amp;10&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>